<commit_message>
basic emission model concept
</commit_message>
<xml_diff>
--- a/tests/fixtures/models/5 - emissions/Concept.xlsx
+++ b/tests/fixtures/models/5 - emissions/Concept.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365.sharepoint.com/sites/documentale-DENG/PRINMIMO/Models/pyESM_docs/concept/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baioc\Documents\GitHub\pyesm\tests\fixtures\models\5 - emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="790" documentId="14_{FAE8ADBD-E4CA-45FB-861B-C036EAC870C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1287625B-42B5-4478-AF68-9DA7166BF017}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C61CA82-F2D2-42AB-B463-5BF3E616DDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C882E439-A7AD-4EB3-AF4A-F0AD2A1D41F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C882E439-A7AD-4EB3-AF4A-F0AD2A1D41F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Emissions" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="90">
   <si>
     <t>PP</t>
   </si>
@@ -316,18 +316,12 @@
     <t>Emissions</t>
   </si>
   <si>
-    <t>Nox</t>
-  </si>
-  <si>
     <t>e_filter</t>
   </si>
   <si>
     <t>t.3.b</t>
   </si>
   <si>
-    <t>Captured_CO2</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
@@ -337,12 +331,6 @@
     <t>E.1</t>
   </si>
   <si>
-    <t>E.2</t>
-  </si>
-  <si>
-    <t>NOx</t>
-  </si>
-  <si>
     <t>CO2_captured</t>
   </si>
   <si>
@@ -373,24 +361,12 @@
     <t>CO2_cap</t>
   </si>
   <si>
-    <t>NOx_int</t>
-  </si>
-  <si>
-    <t>Nox_y</t>
-  </si>
-  <si>
     <t>CO2_tot</t>
   </si>
   <si>
     <t>t.3.a</t>
   </si>
   <si>
-    <t>NOx_tot</t>
-  </si>
-  <si>
-    <t>NOx_cap</t>
-  </si>
-  <si>
     <t>Balances:</t>
   </si>
   <si>
@@ -476,15 +452,58 @@
   </si>
   <si>
     <t>CO2_emitted_int</t>
+  </si>
+  <si>
+    <t>Emissions CO2</t>
+  </si>
+  <si>
+    <t>NG pp</t>
+  </si>
+  <si>
+    <t>NG pp with CCUS</t>
+  </si>
+  <si>
+    <t>c_e</t>
+  </si>
+  <si>
+    <t>e_cap</t>
+  </si>
+  <si>
+    <t>C_e_tot</t>
+  </si>
+  <si>
+    <t>Q'-uX'-Y=0</t>
+  </si>
+  <si>
+    <t>e_f</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>e.1</t>
+  </si>
+  <si>
+    <t>c.1</t>
+  </si>
+  <si>
+    <t>O&amp;M</t>
+  </si>
+  <si>
+    <t>Oil_pp</t>
+  </si>
+  <si>
+    <t>Oil_pp_CCUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -837,7 +856,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -865,7 +884,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -913,6 +931,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -1400,56 +1431,56 @@
   <dimension ref="A1:AN44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="J18" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AE26" sqref="AE26"/>
+      <selection pane="bottomRight" activeCell="AF36" sqref="AF36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="9" width="8.54296875" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" customWidth="1"/>
-    <col min="11" max="14" width="6.81640625" customWidth="1"/>
-    <col min="15" max="15" width="6.26953125" customWidth="1"/>
-    <col min="16" max="16" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="4.81640625" customWidth="1"/>
-    <col min="18" max="21" width="7.453125" customWidth="1"/>
-    <col min="22" max="22" width="12.453125" customWidth="1"/>
-    <col min="23" max="28" width="7.453125" customWidth="1"/>
-    <col min="29" max="30" width="4.81640625" customWidth="1"/>
-    <col min="31" max="31" width="5.26953125" customWidth="1"/>
-    <col min="32" max="32" width="7.1796875" customWidth="1"/>
-    <col min="33" max="33" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.54296875" customWidth="1"/>
-    <col min="35" max="35" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.26953125" customWidth="1"/>
-    <col min="39" max="39" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" customWidth="1"/>
+    <col min="18" max="21" width="7.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1"/>
+    <col min="23" max="28" width="7.42578125" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.28515625" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1488,12 +1519,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="K4" t="s">
@@ -1503,10 +1532,10 @@
         <v>9</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>12</v>
@@ -1522,53 +1551,93 @@
         <v>9</v>
       </c>
       <c r="AE4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AF4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="AA5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
+      <c r="AC5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AK5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
       <c r="P6" s="4"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
@@ -1580,7 +1649,7 @@
       <c r="AF6" s="3"/>
       <c r="AH6" s="4"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="G7" s="5"/>
       <c r="K7" s="5" t="s">
         <v>14</v>
@@ -1591,17 +1660,17 @@
       <c r="R7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="AC7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
@@ -1624,15 +1693,6 @@
       </c>
       <c r="P8" s="6">
         <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W8" t="s">
-        <v>3</v>
       </c>
       <c r="AC8" s="17" cm="1">
         <f t="array" ref="AC8:AF10">MMULT(K8:N10,_xlfn.MUNIT(4)*K30:N30)</f>
@@ -1656,8 +1716,8 @@
         <v>-1.0000000116860974E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
@@ -1680,15 +1740,6 @@
       </c>
       <c r="P9" s="6">
         <v>10</v>
-      </c>
-      <c r="T9" t="s">
-        <v>17</v>
-      </c>
-      <c r="V9" t="s">
-        <v>22</v>
-      </c>
-      <c r="W9" t="s">
-        <v>3</v>
       </c>
       <c r="AC9" s="17">
         <v>0</v>
@@ -1710,8 +1761,8 @@
         <v>1.5799999175669655E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
@@ -1734,15 +1785,6 @@
       </c>
       <c r="P10" s="6">
         <v>10</v>
-      </c>
-      <c r="T10" t="s">
-        <v>23</v>
-      </c>
-      <c r="V10" t="s">
-        <v>24</v>
-      </c>
-      <c r="W10" t="s">
-        <v>3</v>
       </c>
       <c r="AC10" s="17">
         <v>0</v>
@@ -1764,24 +1806,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
       </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
       <c r="G12" s="6">
         <v>1</v>
       </c>
@@ -1793,12 +1838,6 @@
       </c>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="U12" t="s">
-        <v>8</v>
-      </c>
-      <c r="V12" t="s">
-        <v>25</v>
-      </c>
       <c r="Y12" s="17" cm="1">
         <f t="array" ref="Y12:AA14">MMULT(G12:I14,_xlfn.MUNIT(3)*G30:I30)</f>
         <v>44.456401999999997</v>
@@ -1814,13 +1853,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
       </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
       <c r="G13" s="6">
         <v>0</v>
       </c>
@@ -1832,12 +1874,6 @@
       </c>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="U13" t="s">
-        <v>9</v>
-      </c>
-      <c r="V13" t="s">
-        <v>26</v>
-      </c>
       <c r="Y13" s="17">
         <v>0</v>
       </c>
@@ -1851,13 +1887,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
       </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
       <c r="G14" s="6">
         <v>0</v>
       </c>
@@ -1869,12 +1908,6 @@
       </c>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
-      <c r="U14" t="s">
-        <v>10</v>
-      </c>
-      <c r="V14" t="s">
-        <v>27</v>
-      </c>
       <c r="Y14" s="17">
         <v>0</v>
       </c>
@@ -1888,20 +1921,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="R15" s="5"/>
       <c r="AH15" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="C16" s="55" t="s">
+        <v>86</v>
+      </c>
       <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="K16" s="6">
         <v>2</v>
       </c>
@@ -1916,13 +1954,9 @@
       </c>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
-      <c r="V16" t="s">
-        <v>28</v>
-      </c>
-      <c r="W16" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB16" s="7"/>
+      <c r="AB16" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="AC16" s="17" cm="1">
         <f t="array" ref="AC16:AF16">MMULT(K16:N16,_xlfn.MUNIT(4)*K30:N30)</f>
         <v>88.912803999999994</v>
@@ -1936,87 +1970,64 @@
       <c r="AF16" s="17">
         <v>36.588330450000001</v>
       </c>
-      <c r="AH16" s="20">
+      <c r="AH16" s="19">
         <f>SUM(_xlfn.ANCHORARRAY(AC16))</f>
         <v>233.08082159999998</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.35">
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="6">
+    <row r="17" spans="2:40" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="57"/>
+      <c r="J17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="AB17" s="59"/>
+      <c r="AH17" s="60"/>
+    </row>
+    <row r="18" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="6">
         <v>15</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="6">
         <v>15</v>
       </c>
-      <c r="I17" s="6">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="V17" t="s">
-        <v>36</v>
-      </c>
-      <c r="W17" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y17" s="17" cm="1">
-        <f t="array" ref="Y17:AA17">MMULT(G17:I17,_xlfn.MUNIT(3)*G30:I30)</f>
-        <v>666.84602999999993</v>
-      </c>
-      <c r="Z17" s="17">
-        <v>606.22366499999998</v>
-      </c>
-      <c r="AA17" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="7"/>
-    </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.35">
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="6">
-        <v>0</v>
-      </c>
-      <c r="L18" s="6">
-        <v>0</v>
-      </c>
-      <c r="M18" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="N18" s="6">
-        <v>0</v>
-      </c>
-      <c r="V18" t="s">
-        <v>37</v>
-      </c>
-      <c r="W18" t="s">
-        <v>38</v>
-      </c>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="54"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.25">
       <c r="J19" s="7"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" t="s">
-        <v>33</v>
+      <c r="J20" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="K20" s="6">
         <v>0</v>
@@ -2031,10 +2042,10 @@
         <v>0</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -2061,7 +2072,7 @@
         <v>21</v>
       </c>
       <c r="AC21" s="17" cm="1">
-        <f t="array" ref="AC21:AF23">_xlfn.ANCHORARRAY(AC8)*TRANSPOSE(G17:I17)*K25:N27</f>
+        <f t="array" ref="AC21:AF23">_xlfn.ANCHORARRAY(AC8)*TRANSPOSE(G18:I18)*K25:N27</f>
         <v>0</v>
       </c>
       <c r="AD21" s="17">
@@ -2073,22 +2084,22 @@
       <c r="AF21" s="17">
         <v>0</v>
       </c>
-      <c r="AG21" s="29" t="s">
-        <v>41</v>
+      <c r="AG21" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="AH21" s="17" cm="1">
-        <f t="array" ref="AH21:AH23">P8:P10*TRANSPOSE(G17:I17)</f>
-        <v>0</v>
-      </c>
-      <c r="AI21" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ21" s="17">
+        <f t="array" ref="AH21:AH23">P8:P10*TRANSPOSE(G18:I18)</f>
+        <v>0</v>
+      </c>
+      <c r="AI21" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ21" s="45">
         <f>SUM(AC21:AF21) + AH21</f>
         <v>66.684603150000001</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -2126,17 +2137,17 @@
       <c r="AF22" s="17">
         <v>380.51863668000004</v>
       </c>
-      <c r="AG22" s="32"/>
+      <c r="AG22" s="31"/>
       <c r="AH22" s="17">
         <v>150</v>
       </c>
-      <c r="AI22" s="30"/>
-      <c r="AJ22" s="17">
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="45">
         <f>SUM(AC22:AF22) + AH22</f>
         <v>606.22366263000004</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="J23" s="7"/>
       <c r="Z23" t="s">
         <v>23</v>
@@ -2156,32 +2167,32 @@
       <c r="AF23" s="17">
         <v>0</v>
       </c>
-      <c r="AG23" s="30"/>
+      <c r="AG23" s="29"/>
       <c r="AH23" s="17">
         <v>0</v>
       </c>
-      <c r="AI23" s="30"/>
-      <c r="AJ23" s="17">
+      <c r="AI23" s="29"/>
+      <c r="AJ23" s="45">
         <f>SUM(AC23:AF23) + AH23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.25">
       <c r="J24" s="7"/>
-      <c r="AG24" s="30"/>
-      <c r="AI24" s="30"/>
-    </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AG24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="62"/>
+    </row>
+    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="K25" s="6">
         <v>0</v>
       </c>
@@ -2195,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="Y25" s="11"/>
       <c r="Z25" t="s">
@@ -2205,7 +2216,7 @@
         <v>21</v>
       </c>
       <c r="AC25" s="18" cm="1">
-        <f t="array" ref="AC25:AF27">_xlfn.ANCHORARRAY(AC8)*TRANSPOSE(G17:I17)*K20:N22</f>
+        <f t="array" ref="AC25:AF27">_xlfn.ANCHORARRAY(AC8)*TRANSPOSE(G18:I18)*K20:N22</f>
         <v>0</v>
       </c>
       <c r="AD25" s="18">
@@ -2217,10 +2228,11 @@
       <c r="AF25" s="18">
         <v>0</v>
       </c>
-      <c r="AG25" s="30"/>
-      <c r="AI25" s="30"/>
-    </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AG25" s="29"/>
+      <c r="AI25" s="29"/>
+      <c r="AJ25" s="62"/>
+    </row>
+    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>17</v>
       </c>
@@ -2254,10 +2266,11 @@
       <c r="AF26" s="17">
         <v>-372.90826394640004</v>
       </c>
-      <c r="AG26" s="30"/>
-      <c r="AI26" s="30"/>
-    </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AG26" s="29"/>
+      <c r="AI26" s="29"/>
+      <c r="AJ26" s="62"/>
+    </row>
+    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -2291,30 +2304,26 @@
       <c r="AF27" s="17">
         <v>0</v>
       </c>
-      <c r="AG27" s="30"/>
-      <c r="AI27" s="30"/>
-    </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AG27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="62"/>
+    </row>
+    <row r="28" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="P28" s="5"/>
-      <c r="AG28" s="30"/>
+      <c r="AG28" s="29"/>
       <c r="AH28" s="5"/>
-      <c r="AI28" s="30"/>
-    </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.35">
-      <c r="G29" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="AI28" s="29"/>
+      <c r="AJ28" s="62"/>
+    </row>
+    <row r="29" spans="2:40" x14ac:dyDescent="0.25">
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="V29" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="Z29" t="s">
         <v>16</v>
@@ -2335,22 +2344,25 @@
       <c r="AF29" s="17">
         <v>0</v>
       </c>
-      <c r="AG29" s="29" t="s">
-        <v>41</v>
+      <c r="AG29" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="AH29" s="17">
         <f>AH21</f>
         <v>0</v>
       </c>
-      <c r="AI29" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ29" s="17">
+      <c r="AI29" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ29" s="45">
         <f>SUM(AC29:AF29)+AH29</f>
         <v>66.684603150000001</v>
       </c>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="F30" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="G30" s="12">
         <v>44.456401999999997</v>
       </c>
@@ -2360,7 +2372,9 @@
       <c r="I30" s="12">
         <v>10</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="J30" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="K30" s="12">
         <v>44.456401999999997</v>
       </c>
@@ -2392,18 +2406,18 @@
       <c r="AF30" s="17">
         <v>7.610372733600002</v>
       </c>
-      <c r="AG30" s="32"/>
+      <c r="AG30" s="31"/>
       <c r="AH30" s="17">
         <f>AH22</f>
         <v>150</v>
       </c>
-      <c r="AI30" s="30"/>
-      <c r="AJ30" s="17">
+      <c r="AI30" s="29"/>
+      <c r="AJ30" s="45">
         <f t="shared" ref="AJ30:AJ31" si="0">SUM(AC30:AF30)+AH30</f>
         <v>233.31539868359999</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -2430,18 +2444,18 @@
       <c r="AF31" s="17">
         <v>0</v>
       </c>
-      <c r="AG31" s="30"/>
+      <c r="AG31" s="29"/>
       <c r="AH31" s="17">
-        <f t="shared" ref="AH30:AH31" si="1">AH23</f>
-        <v>0</v>
-      </c>
-      <c r="AI31" s="30"/>
-      <c r="AJ31" s="17">
+        <f t="shared" ref="AH31" si="1">AH23</f>
+        <v>0</v>
+      </c>
+      <c r="AI31" s="29"/>
+      <c r="AJ31" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -2450,28 +2464,28 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="P32" s="8"/>
-      <c r="AG32" s="30"/>
-      <c r="AI32" s="30"/>
+      <c r="AG32" s="29"/>
+      <c r="AI32" s="29"/>
       <c r="AM32" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AN32" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="7:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="K33" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="P33" s="8"/>
       <c r="AA33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AC33" s="17">
         <f>SUM(AC29:AC31)</f>
@@ -2489,47 +2503,59 @@
         <f t="shared" si="2"/>
         <v>7.610372733600002</v>
       </c>
-      <c r="AG33" s="30"/>
+      <c r="AG33" s="29"/>
       <c r="AH33" s="17">
         <f>SUM(AH29:AH31)</f>
         <v>150</v>
       </c>
-      <c r="AI33" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ33" s="23">
+      <c r="AI33" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ33" s="22">
         <f>SUM(AJ29:AJ31)/(SUM(AC33:AF33)+AH33)</f>
         <v>1</v>
       </c>
-      <c r="AM33" s="24">
+      <c r="AM33" s="23">
         <f>SUM(AC33:AF33)+AH33</f>
         <v>300.00000183359998</v>
       </c>
-      <c r="AN33" s="25">
+      <c r="AN33" s="24">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="7:40" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="K34" s="21">
+      <c r="K34" s="20">
         <v>1</v>
       </c>
-      <c r="L34" s="21">
-        <v>0</v>
-      </c>
-      <c r="M34" s="21">
-        <v>0</v>
-      </c>
-      <c r="N34" s="21">
+      <c r="L34" s="20">
+        <v>0</v>
+      </c>
+      <c r="M34" s="20">
+        <v>0</v>
+      </c>
+      <c r="N34" s="20">
         <v>0</v>
       </c>
       <c r="P34" s="8"/>
-      <c r="AG34" s="30"/>
-      <c r="AI34" s="30"/>
-    </row>
-    <row r="35" spans="7:40" x14ac:dyDescent="0.35">
+      <c r="AG34" s="29"/>
+      <c r="AI34" s="29"/>
+    </row>
+    <row r="35" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
       <c r="K35" s="13">
         <v>0</v>
       </c>
@@ -2542,207 +2568,104 @@
       <c r="N35" s="13">
         <v>0</v>
       </c>
-      <c r="AG35" s="30"/>
-      <c r="AI35" s="30"/>
-    </row>
-    <row r="36" spans="7:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K36" s="22">
-        <v>0</v>
-      </c>
-      <c r="L36" s="22">
-        <v>0</v>
-      </c>
-      <c r="M36" s="22">
+      <c r="AG35" s="29"/>
+      <c r="AI35" s="29"/>
+    </row>
+    <row r="36" spans="3:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="K36" s="21">
+        <v>0</v>
+      </c>
+      <c r="L36" s="21">
+        <v>0</v>
+      </c>
+      <c r="M36" s="21">
         <v>1</v>
       </c>
-      <c r="N36" s="22">
+      <c r="N36" s="21">
         <v>1</v>
       </c>
       <c r="O36" s="5"/>
       <c r="P36" s="9"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="AG36" s="30"/>
-      <c r="AI36" s="30"/>
-    </row>
-    <row r="37" spans="7:40" x14ac:dyDescent="0.35">
-      <c r="AG37" s="30"/>
-      <c r="AI37" s="30"/>
-    </row>
-    <row r="38" spans="7:40" x14ac:dyDescent="0.35">
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+      <c r="AC36">
+        <v>1</v>
+      </c>
+      <c r="AF36" cm="1">
+        <f t="array" ref="AF36:AF38">MMULT(AC29:AF31,AC36:AC39)</f>
+        <v>66.684603150000001</v>
+      </c>
+      <c r="AH36">
+        <f>SUM(AC29:AF29)</f>
+        <v>66.684603150000001</v>
+      </c>
+    </row>
+    <row r="37" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="AC37">
+        <v>1</v>
+      </c>
+      <c r="AF37">
+        <v>83.315398683600009</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" ref="AH37:AH38" si="3">SUM(AC30:AF30)</f>
+        <v>83.315398683600009</v>
+      </c>
+    </row>
+    <row r="38" spans="3:40" x14ac:dyDescent="0.25">
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
-      <c r="V38" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC38" s="17" cm="1">
-        <f t="array" ref="AC38:AF40">K18:N18*_xlfn.ANCHORARRAY(AC8)</f>
-        <v>0</v>
-      </c>
-      <c r="AD38" s="17">
-        <v>0</v>
-      </c>
-      <c r="AE38" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF38" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG38" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH38" s="17" cm="1">
-        <f t="array" ref="AH38:AH40">TRANSPOSE(MMULT(MMULT(K18:N18,MMULT(TRANSPOSE(K34:N36),G12:I14)),_xlfn.MUNIT(3)*P8:P10))</f>
-        <v>0</v>
-      </c>
-      <c r="AI38" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ38" s="17">
-        <f>SUM(AC38:AF38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="7:40" x14ac:dyDescent="0.35">
+      <c r="AC38">
+        <v>1</v>
+      </c>
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:40" x14ac:dyDescent="0.25">
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
-      <c r="Z39" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA39" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC39" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD39" s="17">
-        <v>0</v>
-      </c>
-      <c r="AE39" s="17">
-        <v>12.617504325000002</v>
-      </c>
-      <c r="AF39" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG39" s="30"/>
-      <c r="AH39" s="17">
-        <v>0</v>
-      </c>
-      <c r="AI39" s="30"/>
-      <c r="AJ39" s="17">
-        <f>SUM(AC39:AF39) + AH39</f>
-        <v>12.617504325000002</v>
-      </c>
-    </row>
-    <row r="40" spans="7:40" x14ac:dyDescent="0.35">
+      <c r="AC39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:40" x14ac:dyDescent="0.25">
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
-      <c r="Z40" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC40" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="17">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF40" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG40" s="30"/>
-      <c r="AH40" s="17">
-        <v>25</v>
-      </c>
-      <c r="AI40" s="30"/>
-      <c r="AJ40" s="17">
-        <f>SUM(AC40:AF40) + AH40</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="7:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="41" spans="3:40" x14ac:dyDescent="0.25">
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
-      <c r="AG41" s="30"/>
-      <c r="AI41" s="30"/>
-      <c r="AM41" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN41" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="7:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="42" spans="3:40" x14ac:dyDescent="0.25">
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
-      <c r="AA42" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC42" s="17">
-        <f>SUM(AC38:AC40)</f>
-        <v>0</v>
-      </c>
-      <c r="AD42" s="17">
-        <f t="shared" ref="AD42:AF42" si="3">SUM(AD38:AD40)</f>
-        <v>0</v>
-      </c>
-      <c r="AE42" s="17">
-        <f t="shared" si="3"/>
-        <v>12.617504325000002</v>
-      </c>
-      <c r="AF42" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG42" s="30"/>
-      <c r="AH42" s="17">
-        <f>SUM(_xlfn.ANCHORARRAY(AH38))</f>
-        <v>25</v>
-      </c>
-      <c r="AI42" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ42" s="23">
-        <f>SUM(AJ38:AJ40)/(SUM(AC42:AF42)+AH42)</f>
-        <v>1</v>
-      </c>
-      <c r="AM42" s="19">
-        <f>SUM(AC40:AF40)+AH40</f>
-        <v>25</v>
-      </c>
-      <c r="AN42" s="25">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="7:40" x14ac:dyDescent="0.35">
-      <c r="AI43" s="30"/>
-    </row>
-    <row r="44" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="54"/>
+    </row>
+    <row r="44" spans="3:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
       <c r="P44" s="5"/>
     </row>
   </sheetData>
@@ -2766,38 +2689,38 @@
       <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="9" width="8.54296875" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" customWidth="1"/>
-    <col min="11" max="14" width="6.81640625" customWidth="1"/>
-    <col min="15" max="15" width="6.26953125" customWidth="1"/>
-    <col min="16" max="16" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="4.81640625" customWidth="1"/>
-    <col min="18" max="21" width="7.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="28" width="7.453125" customWidth="1"/>
-    <col min="29" max="30" width="4.81640625" customWidth="1"/>
-    <col min="31" max="31" width="5.26953125" customWidth="1"/>
-    <col min="32" max="32" width="7.1796875" customWidth="1"/>
-    <col min="33" max="33" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.54296875" customWidth="1"/>
-    <col min="35" max="35" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="14" width="6.85546875" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" customWidth="1"/>
+    <col min="18" max="21" width="7.42578125" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="7.42578125" customWidth="1"/>
+    <col min="29" max="30" width="4.85546875" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.26953125" customWidth="1"/>
-    <col min="39" max="39" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.81640625" customWidth="1"/>
+    <col min="37" max="38" width="5.28515625" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2806,7 +2729,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -2824,10 +2747,10 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2843,13 +2766,13 @@
         <v>23</v>
       </c>
       <c r="AE3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AF3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -2864,10 +2787,10 @@
         <v>9</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>12</v>
@@ -2883,16 +2806,16 @@
         <v>9</v>
       </c>
       <c r="AE4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AF4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2915,10 +2838,10 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AK5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2941,7 +2864,7 @@
       <c r="AF6" s="3"/>
       <c r="AH6" s="4"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="G7" s="5"/>
       <c r="K7" s="5" t="s">
         <v>14</v>
@@ -2952,21 +2875,21 @@
       <c r="R7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="AC7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -2990,7 +2913,7 @@
         <v>16</v>
       </c>
       <c r="V8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="W8" t="s">
         <v>3</v>
@@ -3016,12 +2939,12 @@
         <v>9.9999999392252903E-8</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -3045,7 +2968,7 @@
         <v>17</v>
       </c>
       <c r="V9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="W9" t="s">
         <v>3</v>
@@ -3070,12 +2993,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -3099,7 +3022,7 @@
         <v>23</v>
       </c>
       <c r="V10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="W10" t="s">
         <v>3</v>
@@ -3124,23 +3047,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -3160,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="V12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="W12" t="s">
         <v>3</v>
@@ -3180,12 +3103,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -3205,7 +3128,7 @@
         <v>9</v>
       </c>
       <c r="V13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="W13" t="s">
         <v>3</v>
@@ -3223,12 +3146,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -3248,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="V14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="W14" t="s">
         <v>3</v>
@@ -3266,19 +3189,19 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="R15" s="5"/>
       <c r="AH15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AM15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>28</v>
       </c>
@@ -3320,15 +3243,15 @@
       <c r="AF16" s="17">
         <v>0</v>
       </c>
-      <c r="AH16" s="20">
+      <c r="AH16" s="19">
         <f>SUM(_xlfn.ANCHORARRAY(AC16))</f>
         <v>45.277777999999998</v>
       </c>
-      <c r="AM16" s="28">
+      <c r="AM16" s="27">
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>29</v>
       </c>
@@ -3341,12 +3264,12 @@
       <c r="H17" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="43">
         <v>0</v>
       </c>
       <c r="J17" s="7"/>
       <c r="V17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="W17" t="s">
         <v>5</v>
@@ -3362,44 +3285,44 @@
         <v>0</v>
       </c>
       <c r="AB17" s="7"/>
-      <c r="AM17" s="28">
+      <c r="AM17" s="27">
         <f>AM16*AA14</f>
         <v>3</v>
       </c>
       <c r="AN17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:40" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.25">
       <c r="J19" s="7"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="AC20" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AH20" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="6">
@@ -3418,7 +3341,7 @@
         <v>16</v>
       </c>
       <c r="AA21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AC21" s="17" cm="1">
         <f t="array" ref="AC21:AF23">_xlfn.ANCHORARRAY(AC8)*TRANSPOSE(G17:I17)*K21:N23</f>
@@ -3442,12 +3365,12 @@
         <v>283.33333349999998</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K22" s="6">
         <v>0</v>
@@ -3465,7 +3388,7 @@
         <v>17</v>
       </c>
       <c r="AA22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AC22" s="17">
         <v>0</v>
@@ -3488,12 +3411,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K23" s="6">
         <v>0</v>
@@ -3511,7 +3434,7 @@
         <v>23</v>
       </c>
       <c r="AA23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AC23" s="17">
         <v>0</v>
@@ -3533,18 +3456,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="AM24" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AN24" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G25" s="5" t="s">
         <v>19</v>
       </c>
@@ -3555,7 +3478,7 @@
         <v>20</v>
       </c>
       <c r="AA25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AC25" s="17">
         <f>SUM(AC21:AC23)</f>
@@ -3577,22 +3500,22 @@
         <f>SUM(_xlfn.ANCHORARRAY(AH21))</f>
         <v>150</v>
       </c>
-      <c r="AI25" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ25" s="23">
+      <c r="AI25" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ25" s="22">
         <f>SUM(AJ21:AJ23)/(SUM(AC25:AF25)+AH25)</f>
         <v>1</v>
       </c>
-      <c r="AM25" s="24">
+      <c r="AM25" s="23">
         <f>SUM(AC25:AF25)+AH25</f>
         <v>283.33333349999998</v>
       </c>
-      <c r="AN25" s="25">
+      <c r="AN25" s="24">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G26" s="12">
         <v>18.888888999999999</v>
       </c>
@@ -3616,7 +3539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -3624,24 +3547,24 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="34"/>
-      <c r="AA27" s="34"/>
-      <c r="AB27" s="34"/>
-      <c r="AC27" s="34"/>
-      <c r="AD27" s="34"/>
-      <c r="AE27" s="34"/>
-      <c r="AF27" s="34"/>
-      <c r="AG27" s="34"/>
-      <c r="AH27" s="34"/>
-      <c r="AI27" s="34"/>
-      <c r="AJ27" s="34"/>
-      <c r="AK27" s="34"/>
-      <c r="AL27" s="34"/>
-      <c r="AM27" s="34"/>
-      <c r="AN27" s="35"/>
-    </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="33"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="33"/>
+      <c r="AD27" s="33"/>
+      <c r="AE27" s="33"/>
+      <c r="AF27" s="33"/>
+      <c r="AG27" s="33"/>
+      <c r="AH27" s="33"/>
+      <c r="AI27" s="33"/>
+      <c r="AJ27" s="33"/>
+      <c r="AK27" s="33"/>
+      <c r="AL27" s="33"/>
+      <c r="AM27" s="33"/>
+      <c r="AN27" s="34"/>
+    </row>
+    <row r="28" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -3650,57 +3573,57 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="P28" s="5"/>
-      <c r="Y28" s="36" t="s">
-        <v>70</v>
+      <c r="Y28" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
-      <c r="AN28" s="37"/>
-    </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AN28" s="36"/>
+    </row>
+    <row r="29" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="K29" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="Y29" s="38"/>
+      <c r="Y29" s="37"/>
       <c r="AJ29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AM29" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN29" s="39"/>
-    </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="AN29" s="38"/>
+    </row>
+    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="K30" s="21">
+      <c r="K30" s="20">
         <v>1</v>
       </c>
-      <c r="L30" s="21">
-        <v>0</v>
-      </c>
-      <c r="M30" s="21">
-        <v>0</v>
-      </c>
-      <c r="N30" s="21">
+      <c r="L30" s="20">
+        <v>0</v>
+      </c>
+      <c r="M30" s="20">
+        <v>0</v>
+      </c>
+      <c r="N30" s="20">
         <v>0</v>
       </c>
       <c r="P30" s="8"/>
       <c r="V30" s="5"/>
-      <c r="Y30" s="38"/>
+      <c r="Y30" s="37"/>
       <c r="Z30" t="s">
         <v>16</v>
       </c>
       <c r="AA30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AC30" s="17">
         <f>AC21</f>
@@ -3726,13 +3649,13 @@
         <f>SUM(AC30:AH30)</f>
         <v>178.33333350000001</v>
       </c>
-      <c r="AM30" s="28">
+      <c r="AM30" s="27">
         <f>(G17*M26+H17*N26)/(M26+N26)</f>
         <v>10.5</v>
       </c>
-      <c r="AN30" s="37"/>
-    </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AN30" s="36"/>
+    </row>
+    <row r="31" spans="2:40" x14ac:dyDescent="0.25">
       <c r="K31" s="13">
         <v>0</v>
       </c>
@@ -3746,12 +3669,12 @@
         <v>0</v>
       </c>
       <c r="P31" s="8"/>
-      <c r="Y31" s="38"/>
+      <c r="Y31" s="37"/>
       <c r="Z31" t="s">
         <v>17</v>
       </c>
       <c r="AA31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AC31" s="17">
         <f>AC22</f>
@@ -3775,9 +3698,9 @@
         <f t="shared" ref="AJ31:AJ32" si="0">SUM(AC31:AH31)</f>
         <v>0</v>
       </c>
-      <c r="AN31" s="37"/>
-    </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AN31" s="36"/>
+    </row>
+    <row r="32" spans="2:40" x14ac:dyDescent="0.25">
       <c r="K32" s="13">
         <v>0</v>
       </c>
@@ -3791,12 +3714,12 @@
         <v>1</v>
       </c>
       <c r="P32" s="8"/>
-      <c r="Y32" s="38"/>
+      <c r="Y32" s="37"/>
       <c r="Z32" t="s">
         <v>23</v>
       </c>
       <c r="AA32" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AC32" s="17">
         <v>0</v>
@@ -3818,23 +3741,23 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="AN32" s="37"/>
-    </row>
-    <row r="33" spans="11:40" x14ac:dyDescent="0.35">
+      <c r="AN32" s="36"/>
+    </row>
+    <row r="33" spans="11:40" x14ac:dyDescent="0.25">
       <c r="P33" s="8"/>
-      <c r="Y33" s="38"/>
+      <c r="Y33" s="37"/>
       <c r="AM33" s="5"/>
-      <c r="AN33" s="39"/>
-    </row>
-    <row r="34" spans="11:40" x14ac:dyDescent="0.35">
+      <c r="AN33" s="38"/>
+    </row>
+    <row r="34" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="P34" s="8"/>
-      <c r="Y34" s="38"/>
+      <c r="Y34" s="37"/>
       <c r="AB34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="AC34" s="17">
         <f>SUM(AC30:AC32)</f>
@@ -3860,63 +3783,63 @@
         <f t="shared" si="1"/>
         <v>255</v>
       </c>
-      <c r="AI34" s="27"/>
-      <c r="AJ34" s="26"/>
-      <c r="AN34" s="40"/>
-    </row>
-    <row r="35" spans="11:40" x14ac:dyDescent="0.35">
-      <c r="Y35" s="41"/>
-      <c r="Z35" s="42"/>
-      <c r="AA35" s="42"/>
-      <c r="AB35" s="42"/>
-      <c r="AC35" s="42"/>
-      <c r="AD35" s="42"/>
-      <c r="AE35" s="42"/>
-      <c r="AF35" s="42"/>
-      <c r="AG35" s="42"/>
-      <c r="AH35" s="42"/>
-      <c r="AI35" s="42"/>
-      <c r="AJ35" s="42"/>
-      <c r="AK35" s="42"/>
-      <c r="AL35" s="42"/>
-      <c r="AM35" s="42"/>
-      <c r="AN35" s="43"/>
-    </row>
-    <row r="36" spans="11:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AI34" s="26"/>
+      <c r="AJ34" s="25"/>
+      <c r="AN34" s="39"/>
+    </row>
+    <row r="35" spans="11:40" x14ac:dyDescent="0.25">
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="41"/>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="41"/>
+      <c r="AD35" s="41"/>
+      <c r="AE35" s="41"/>
+      <c r="AF35" s="41"/>
+      <c r="AG35" s="41"/>
+      <c r="AH35" s="41"/>
+      <c r="AI35" s="41"/>
+      <c r="AJ35" s="41"/>
+      <c r="AK35" s="41"/>
+      <c r="AL35" s="41"/>
+      <c r="AM35" s="41"/>
+      <c r="AN35" s="42"/>
+    </row>
+    <row r="36" spans="11:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O36" s="5"/>
       <c r="P36" s="9"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-    </row>
-    <row r="39" spans="11:40" x14ac:dyDescent="0.35">
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+    </row>
+    <row r="39" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
     </row>
-    <row r="40" spans="11:40" x14ac:dyDescent="0.35">
+    <row r="40" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
     </row>
-    <row r="41" spans="11:40" x14ac:dyDescent="0.35">
+    <row r="41" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
     </row>
-    <row r="42" spans="11:40" x14ac:dyDescent="0.35">
+    <row r="42" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
     </row>
-    <row r="44" spans="11:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="54"/>
+    <row r="44" spans="11:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
       <c r="P44" s="5"/>
     </row>
   </sheetData>
@@ -3940,38 +3863,38 @@
       <selection pane="bottomRight" activeCell="AN19" sqref="AN19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="9" width="8.54296875" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" customWidth="1"/>
-    <col min="11" max="14" width="6.81640625" customWidth="1"/>
-    <col min="15" max="15" width="6.26953125" customWidth="1"/>
-    <col min="16" max="16" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="4.81640625" customWidth="1"/>
-    <col min="18" max="21" width="7.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="28" width="7.453125" customWidth="1"/>
-    <col min="29" max="30" width="4.81640625" customWidth="1"/>
-    <col min="31" max="31" width="5.26953125" customWidth="1"/>
-    <col min="32" max="32" width="7.1796875" customWidth="1"/>
-    <col min="33" max="33" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.54296875" customWidth="1"/>
-    <col min="35" max="35" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="14" width="6.85546875" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" customWidth="1"/>
+    <col min="18" max="21" width="7.42578125" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="7.42578125" customWidth="1"/>
+    <col min="29" max="30" width="4.85546875" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.26953125" customWidth="1"/>
-    <col min="39" max="39" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.81640625" customWidth="1"/>
+    <col min="37" max="38" width="5.28515625" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3980,7 +3903,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -3998,10 +3921,10 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -4017,13 +3940,13 @@
         <v>23</v>
       </c>
       <c r="AE3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AF3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -4038,10 +3961,10 @@
         <v>9</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>12</v>
@@ -4057,16 +3980,16 @@
         <v>9</v>
       </c>
       <c r="AE4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AF4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4089,10 +4012,10 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AL5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4115,7 +4038,7 @@
       <c r="AF6" s="3"/>
       <c r="AH6" s="4"/>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="G7" s="5"/>
       <c r="K7" s="5" t="s">
         <v>14</v>
@@ -4126,7 +4049,7 @@
       <c r="R7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="AC7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH7" s="5" t="s">
         <v>15</v>
@@ -4135,15 +4058,15 @@
         <v>19</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -4167,7 +4090,7 @@
         <v>16</v>
       </c>
       <c r="V8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="W8" t="s">
         <v>3</v>
@@ -4188,7 +4111,7 @@
       <c r="AH8" s="6">
         <v>10</v>
       </c>
-      <c r="AJ8" s="46" cm="1">
+      <c r="AJ8" s="45" cm="1">
         <f t="array" ref="AJ8:AJ10">TRANSPOSE(G26:I26)</f>
         <v>20</v>
       </c>
@@ -4197,12 +4120,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -4226,7 +4149,7 @@
         <v>17</v>
       </c>
       <c r="V9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="W9" t="s">
         <v>3</v>
@@ -4247,19 +4170,19 @@
         <f>P9</f>
         <v>0</v>
       </c>
-      <c r="AJ9" s="46">
+      <c r="AJ9" s="45">
         <v>2</v>
       </c>
       <c r="AL9" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -4283,7 +4206,7 @@
         <v>23</v>
       </c>
       <c r="V10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="W10" t="s">
         <v>3</v>
@@ -4304,33 +4227,33 @@
         <f>P10</f>
         <v>10</v>
       </c>
-      <c r="AJ10" s="46">
+      <c r="AJ10" s="45">
         <v>10</v>
       </c>
       <c r="AL10" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -4350,7 +4273,7 @@
         <v>8</v>
       </c>
       <c r="V12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="W12" t="s">
         <v>3</v>
@@ -4365,7 +4288,7 @@
       <c r="AA12" s="17">
         <v>0</v>
       </c>
-      <c r="AJ12" s="46" cm="1">
+      <c r="AJ12" s="45" cm="1">
         <f t="array" ref="AJ12:AJ14">MMULT(K30:N32, TRANSPOSE(K26:N26))</f>
         <v>20</v>
       </c>
@@ -4374,12 +4297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -4399,7 +4322,7 @@
         <v>9</v>
       </c>
       <c r="V13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="W13" t="s">
         <v>3</v>
@@ -4413,19 +4336,19 @@
       <c r="AA13" s="17">
         <v>0</v>
       </c>
-      <c r="AJ13" s="46">
+      <c r="AJ13" s="45">
         <v>2</v>
       </c>
       <c r="AL13" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -4445,7 +4368,7 @@
         <v>10</v>
       </c>
       <c r="V14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="W14" t="s">
         <v>3</v>
@@ -4456,26 +4379,26 @@
       <c r="Z14" s="17">
         <v>0</v>
       </c>
-      <c r="AA14" s="48">
+      <c r="AA14" s="47">
         <v>10</v>
       </c>
-      <c r="AJ14" s="46">
+      <c r="AJ14" s="45">
         <v>10</v>
       </c>
       <c r="AL14" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="R15" s="5"/>
       <c r="AH15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AN15" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>28</v>
       </c>
@@ -4517,15 +4440,15 @@
       <c r="AF16" s="17">
         <v>0</v>
       </c>
-      <c r="AH16" s="20">
+      <c r="AH16" s="19">
         <f>SUM(_xlfn.ANCHORARRAY(AC16))</f>
         <v>45</v>
       </c>
-      <c r="AN16" s="49">
+      <c r="AN16" s="48">
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:41" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>29</v>
       </c>
@@ -4538,12 +4461,12 @@
       <c r="H17" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="43">
         <v>0</v>
       </c>
       <c r="J17" s="7"/>
       <c r="V17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="W17" t="s">
         <v>5</v>
@@ -4560,43 +4483,43 @@
       </c>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="AB18" s="7"/>
       <c r="AN18" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J19" s="7"/>
       <c r="AB19" s="7"/>
-      <c r="AN19" s="50">
+      <c r="AN19" s="49">
         <f>N26/M26</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:41" x14ac:dyDescent="0.25">
       <c r="AC20" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AH20" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AK20" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="6">
@@ -4615,7 +4538,7 @@
         <v>16</v>
       </c>
       <c r="AA21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AC21" s="17" cm="1">
         <f t="array" ref="AC21:AF23">_xlfn.ANCHORARRAY(AC8)*TRANSPOSE(G17:I17)*K21:N23</f>
@@ -4639,12 +4562,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K22" s="6">
         <v>0</v>
@@ -4662,7 +4585,7 @@
         <v>17</v>
       </c>
       <c r="AA22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AC22" s="17">
         <v>0</v>
@@ -4685,12 +4608,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K23" s="6">
         <v>0</v>
@@ -4708,7 +4631,7 @@
         <v>23</v>
       </c>
       <c r="AA23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AC23" s="17">
         <v>0</v>
@@ -4730,18 +4653,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="AN24" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AO24" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G25" s="5" t="s">
         <v>19</v>
       </c>
@@ -4752,7 +4675,7 @@
         <v>20</v>
       </c>
       <c r="AA25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AC25" s="17">
         <f>SUM(AC21:AC23)</f>
@@ -4774,22 +4697,22 @@
         <f>SUM(_xlfn.ANCHORARRAY(AH21))</f>
         <v>150</v>
       </c>
-      <c r="AJ25" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK25" s="23">
+      <c r="AJ25" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK25" s="22">
         <f>SUM(AK21:AK23)/(SUM(AC25:AF25)+AH25)</f>
         <v>1</v>
       </c>
-      <c r="AN25" s="24">
+      <c r="AN25" s="23">
         <f>SUM(AC25:AF25)+AH25</f>
         <v>300</v>
       </c>
-      <c r="AO25" s="25">
+      <c r="AO25" s="24">
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:41" x14ac:dyDescent="0.25">
       <c r="G26" s="12">
         <v>20</v>
       </c>
@@ -4813,95 +4736,95 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="L27" s="8"/>
-      <c r="M27" s="47" t="s">
-        <v>78</v>
+      <c r="M27" s="46" t="s">
+        <v>70</v>
       </c>
       <c r="N27" s="8"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="34"/>
-      <c r="AA27" s="34"/>
-      <c r="AB27" s="34"/>
-      <c r="AC27" s="34"/>
-      <c r="AD27" s="34"/>
-      <c r="AE27" s="34"/>
-      <c r="AF27" s="34"/>
-      <c r="AG27" s="34"/>
-      <c r="AH27" s="34"/>
-      <c r="AI27" s="34"/>
-      <c r="AJ27" s="34"/>
-      <c r="AK27" s="34"/>
-      <c r="AL27" s="34"/>
-      <c r="AM27" s="34"/>
-      <c r="AN27" s="35"/>
-    </row>
-    <row r="28" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="33"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="33"/>
+      <c r="AD27" s="33"/>
+      <c r="AE27" s="33"/>
+      <c r="AF27" s="33"/>
+      <c r="AG27" s="33"/>
+      <c r="AH27" s="33"/>
+      <c r="AI27" s="33"/>
+      <c r="AJ27" s="33"/>
+      <c r="AK27" s="33"/>
+      <c r="AL27" s="33"/>
+      <c r="AM27" s="33"/>
+      <c r="AN27" s="34"/>
+    </row>
+    <row r="28" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
-      <c r="N28" s="51">
+      <c r="N28" s="50">
         <f>AA14*AN16</f>
         <v>3</v>
       </c>
       <c r="P28" s="5"/>
-      <c r="Y28" s="36" t="s">
-        <v>70</v>
+      <c r="Y28" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
-      <c r="AN28" s="37"/>
-    </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.35">
+      <c r="AN28" s="36"/>
+    </row>
+    <row r="29" spans="2:41" x14ac:dyDescent="0.25">
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="K29" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="Y29" s="38"/>
+      <c r="Y29" s="37"/>
       <c r="AJ29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AM29" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN29" s="39"/>
-    </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="AN29" s="38"/>
+    </row>
+    <row r="30" spans="2:41" x14ac:dyDescent="0.25">
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="K30" s="21">
+      <c r="K30" s="20">
         <v>1</v>
       </c>
-      <c r="L30" s="21">
-        <v>0</v>
-      </c>
-      <c r="M30" s="21">
-        <v>0</v>
-      </c>
-      <c r="N30" s="21">
+      <c r="L30" s="20">
+        <v>0</v>
+      </c>
+      <c r="M30" s="20">
+        <v>0</v>
+      </c>
+      <c r="N30" s="20">
         <v>0</v>
       </c>
       <c r="P30" s="8"/>
       <c r="V30" s="5"/>
-      <c r="Y30" s="38"/>
+      <c r="Y30" s="37"/>
       <c r="Z30" t="s">
         <v>16</v>
       </c>
       <c r="AA30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AC30" s="17">
         <f>AC21</f>
@@ -4927,13 +4850,13 @@
         <f>SUM(AC30:AH30)</f>
         <v>180</v>
       </c>
-      <c r="AM30" s="52">
+      <c r="AM30" s="51">
         <f>(G17*M26+H17*N26)/(M26+N26)</f>
         <v>12</v>
       </c>
-      <c r="AN30" s="37"/>
-    </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.35">
+      <c r="AN30" s="36"/>
+    </row>
+    <row r="31" spans="2:41" x14ac:dyDescent="0.25">
       <c r="K31" s="13">
         <v>0</v>
       </c>
@@ -4947,12 +4870,12 @@
         <v>0</v>
       </c>
       <c r="P31" s="8"/>
-      <c r="Y31" s="38"/>
+      <c r="Y31" s="37"/>
       <c r="Z31" t="s">
         <v>17</v>
       </c>
       <c r="AA31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AC31" s="17">
         <f>AC22</f>
@@ -4976,9 +4899,9 @@
         <f t="shared" ref="AJ31:AJ32" si="0">SUM(AC31:AH31)</f>
         <v>0</v>
       </c>
-      <c r="AN31" s="37"/>
-    </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.35">
+      <c r="AN31" s="36"/>
+    </row>
+    <row r="32" spans="2:41" x14ac:dyDescent="0.25">
       <c r="K32" s="13">
         <v>0</v>
       </c>
@@ -4992,12 +4915,12 @@
         <v>1</v>
       </c>
       <c r="P32" s="8"/>
-      <c r="Y32" s="38"/>
+      <c r="Y32" s="37"/>
       <c r="Z32" t="s">
         <v>23</v>
       </c>
       <c r="AA32" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AC32" s="17">
         <v>0</v>
@@ -5019,23 +4942,23 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="AN32" s="37"/>
-    </row>
-    <row r="33" spans="11:40" x14ac:dyDescent="0.35">
+      <c r="AN32" s="36"/>
+    </row>
+    <row r="33" spans="11:40" x14ac:dyDescent="0.25">
       <c r="P33" s="8"/>
-      <c r="Y33" s="38"/>
+      <c r="Y33" s="37"/>
       <c r="AM33" s="5"/>
-      <c r="AN33" s="39"/>
-    </row>
-    <row r="34" spans="11:40" x14ac:dyDescent="0.35">
+      <c r="AN33" s="38"/>
+    </row>
+    <row r="34" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="P34" s="8"/>
-      <c r="Y34" s="38"/>
+      <c r="Y34" s="37"/>
       <c r="AB34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="AC34" s="17">
         <f>SUM(AC30:AC32)</f>
@@ -5061,63 +4984,63 @@
         <f t="shared" si="1"/>
         <v>270</v>
       </c>
-      <c r="AI34" s="27"/>
-      <c r="AJ34" s="26"/>
-      <c r="AN34" s="40"/>
-    </row>
-    <row r="35" spans="11:40" x14ac:dyDescent="0.35">
-      <c r="Y35" s="41"/>
-      <c r="Z35" s="42"/>
-      <c r="AA35" s="42"/>
-      <c r="AB35" s="42"/>
-      <c r="AC35" s="42"/>
-      <c r="AD35" s="42"/>
-      <c r="AE35" s="42"/>
-      <c r="AF35" s="42"/>
-      <c r="AG35" s="42"/>
-      <c r="AH35" s="42"/>
-      <c r="AI35" s="42"/>
-      <c r="AJ35" s="42"/>
-      <c r="AK35" s="42"/>
-      <c r="AL35" s="42"/>
-      <c r="AM35" s="42"/>
-      <c r="AN35" s="43"/>
-    </row>
-    <row r="36" spans="11:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AI34" s="26"/>
+      <c r="AJ34" s="25"/>
+      <c r="AN34" s="39"/>
+    </row>
+    <row r="35" spans="11:40" x14ac:dyDescent="0.25">
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="41"/>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="41"/>
+      <c r="AD35" s="41"/>
+      <c r="AE35" s="41"/>
+      <c r="AF35" s="41"/>
+      <c r="AG35" s="41"/>
+      <c r="AH35" s="41"/>
+      <c r="AI35" s="41"/>
+      <c r="AJ35" s="41"/>
+      <c r="AK35" s="41"/>
+      <c r="AL35" s="41"/>
+      <c r="AM35" s="41"/>
+      <c r="AN35" s="42"/>
+    </row>
+    <row r="36" spans="11:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O36" s="5"/>
       <c r="P36" s="9"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-    </row>
-    <row r="39" spans="11:40" x14ac:dyDescent="0.35">
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+    </row>
+    <row r="39" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
     </row>
-    <row r="40" spans="11:40" x14ac:dyDescent="0.35">
+    <row r="40" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
     </row>
-    <row r="41" spans="11:40" x14ac:dyDescent="0.35">
+    <row r="41" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
     </row>
-    <row r="42" spans="11:40" x14ac:dyDescent="0.35">
+    <row r="42" spans="11:40" x14ac:dyDescent="0.25">
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
     </row>
-    <row r="44" spans="11:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="54"/>
+    <row r="44" spans="11:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
       <c r="P44" s="5"/>
     </row>
   </sheetData>
@@ -5141,38 +5064,38 @@
       <selection pane="bottomRight" activeCell="AW30" sqref="AW30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="10" width="8.54296875" customWidth="1"/>
-    <col min="11" max="11" width="4.7265625" customWidth="1"/>
-    <col min="12" max="16" width="6.81640625" customWidth="1"/>
-    <col min="17" max="17" width="6.26953125" customWidth="1"/>
-    <col min="18" max="18" width="9.453125" customWidth="1"/>
-    <col min="19" max="19" width="4.81640625" customWidth="1"/>
-    <col min="20" max="23" width="7.453125" customWidth="1"/>
-    <col min="24" max="24" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="31" width="7.453125" customWidth="1"/>
-    <col min="32" max="33" width="4.81640625" customWidth="1"/>
-    <col min="34" max="34" width="5.26953125" customWidth="1"/>
-    <col min="35" max="35" width="7.1796875" customWidth="1"/>
-    <col min="36" max="36" width="6.81640625" customWidth="1"/>
-    <col min="37" max="38" width="9.54296875" customWidth="1"/>
-    <col min="39" max="39" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="16" width="6.85546875" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" customWidth="1"/>
+    <col min="20" max="23" width="7.42578125" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="31" width="7.42578125" customWidth="1"/>
+    <col min="32" max="33" width="4.85546875" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" customWidth="1"/>
+    <col min="35" max="35" width="7.140625" customWidth="1"/>
+    <col min="36" max="36" width="6.85546875" customWidth="1"/>
+    <col min="37" max="38" width="9.5703125" customWidth="1"/>
+    <col min="39" max="39" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="10" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="5.26953125" customWidth="1"/>
-    <col min="43" max="43" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.81640625" customWidth="1"/>
+    <col min="41" max="42" width="5.28515625" customWidth="1"/>
+    <col min="43" max="43" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -5181,7 +5104,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -5199,13 +5122,13 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="O3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -5221,16 +5144,16 @@
         <v>23</v>
       </c>
       <c r="AD3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="AH3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AI3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -5245,13 +5168,13 @@
         <v>9</v>
       </c>
       <c r="N4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>12</v>
@@ -5267,19 +5190,19 @@
         <v>9</v>
       </c>
       <c r="AH4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AI4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AJ4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="AL4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -5305,10 +5228,10 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AP5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -5332,7 +5255,7 @@
       <c r="AI6" s="3"/>
       <c r="AL6" s="4"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="G7" s="5"/>
       <c r="L7" s="5" t="s">
         <v>14</v>
@@ -5343,7 +5266,7 @@
       <c r="T7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AF7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AL7" s="5" t="s">
         <v>15</v>
@@ -5352,15 +5275,15 @@
         <v>19</v>
       </c>
       <c r="AP7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -5387,7 +5310,7 @@
         <v>16</v>
       </c>
       <c r="X8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="Y8" t="s">
         <v>3</v>
@@ -5411,7 +5334,7 @@
       <c r="AL8" s="6">
         <v>10</v>
       </c>
-      <c r="AN8" s="46" cm="1">
+      <c r="AN8" s="45" cm="1">
         <f t="array" ref="AN8:AN11">TRANSPOSE(G29:J29)</f>
         <v>0</v>
       </c>
@@ -5420,12 +5343,12 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -5452,7 +5375,7 @@
         <v>17</v>
       </c>
       <c r="X9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="Y9" t="s">
         <v>3</v>
@@ -5476,19 +5399,19 @@
         <f>R9</f>
         <v>0</v>
       </c>
-      <c r="AN9" s="46">
+      <c r="AN9" s="45">
         <v>0</v>
       </c>
       <c r="AP9" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -5515,7 +5438,7 @@
         <v>23</v>
       </c>
       <c r="X10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="Y10" t="s">
         <v>3</v>
@@ -5539,19 +5462,19 @@
         <f>R10</f>
         <v>0</v>
       </c>
-      <c r="AN10" s="46">
+      <c r="AN10" s="45">
         <v>0</v>
       </c>
       <c r="AP10" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -5575,10 +5498,10 @@
         <v>10</v>
       </c>
       <c r="W11" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="X11" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="Y11" t="s">
         <v>3</v>
@@ -5602,33 +5525,33 @@
         <f>R11</f>
         <v>10</v>
       </c>
-      <c r="AN11" s="46">
+      <c r="AN11" s="45">
         <v>0</v>
       </c>
       <c r="AP11" s="16">
         <v>-10</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="G12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="AA12" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AN12" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="AP12" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -5651,7 +5574,7 @@
         <v>8</v>
       </c>
       <c r="X13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="Y13" t="s">
         <v>3</v>
@@ -5669,7 +5592,7 @@
       <c r="AD13" s="17">
         <v>0</v>
       </c>
-      <c r="AN13" s="46" cm="1">
+      <c r="AN13" s="45" cm="1">
         <f t="array" ref="AN13:AN16">MMULT(L33:P36, TRANSPOSE(L29:P29))</f>
         <v>0</v>
       </c>
@@ -5678,12 +5601,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -5706,7 +5629,7 @@
         <v>9</v>
       </c>
       <c r="X14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Y14" t="s">
         <v>3</v>
@@ -5723,19 +5646,19 @@
       <c r="AD14" s="17">
         <v>0</v>
       </c>
-      <c r="AN14" s="46">
+      <c r="AN14" s="45">
         <v>0</v>
       </c>
       <c r="AP14" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -5758,7 +5681,7 @@
         <v>10</v>
       </c>
       <c r="X15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="Y15" t="s">
         <v>3</v>
@@ -5769,25 +5692,25 @@
       <c r="AB15" s="17">
         <v>0</v>
       </c>
-      <c r="AC15" s="48">
+      <c r="AC15" s="47">
         <v>0</v>
       </c>
       <c r="AD15" s="17">
         <v>0</v>
       </c>
-      <c r="AN15" s="46">
+      <c r="AN15" s="45">
         <v>0</v>
       </c>
       <c r="AP15" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -5804,10 +5727,10 @@
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
       <c r="W16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="X16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="Y16" t="s">
         <v>3</v>
@@ -5824,23 +5747,23 @@
       <c r="AD16" s="17">
         <v>0</v>
       </c>
-      <c r="AN16" s="46">
+      <c r="AN16" s="45">
         <v>0</v>
       </c>
       <c r="AP16" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:45" x14ac:dyDescent="0.25">
       <c r="T17" s="5"/>
       <c r="AL17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AR17" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="2:45" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:45" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>28</v>
       </c>
@@ -5888,15 +5811,15 @@
       <c r="AJ18" s="17">
         <v>0</v>
       </c>
-      <c r="AL18" s="20">
+      <c r="AL18" s="19">
         <f>SUM(_xlfn.ANCHORARRAY(AF18))</f>
         <v>0</v>
       </c>
-      <c r="AR18" s="49">
+      <c r="AR18" s="48">
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:45" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>29</v>
       </c>
@@ -5912,12 +5835,12 @@
       <c r="I19" s="6">
         <v>0</v>
       </c>
-      <c r="J19" s="53">
+      <c r="J19" s="52">
         <v>0</v>
       </c>
       <c r="K19" s="7"/>
       <c r="X19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y19" t="s">
         <v>5</v>
@@ -5937,44 +5860,44 @@
       </c>
       <c r="AE19" s="7"/>
     </row>
-    <row r="20" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AE20" s="7"/>
       <c r="AR20" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J21" t="e">
         <f>G19-J19*(1+AR21)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K21" s="7"/>
       <c r="AE21" s="7"/>
-      <c r="AR21" s="50" t="e">
+      <c r="AR21" s="49" t="e">
         <f>O29/N29</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:45" x14ac:dyDescent="0.25">
       <c r="AF22" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="AL22" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AO22" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="2:45" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="6">
@@ -5996,7 +5919,7 @@
         <v>16</v>
       </c>
       <c r="AC23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AF23" s="17" cm="1">
         <f t="array" ref="AF23:AJ26">_xlfn.ANCHORARRAY(AF8)*TRANSPOSE(G19:J19)*L23:P26</f>
@@ -6023,12 +5946,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="L24" s="6">
         <v>0</v>
@@ -6049,7 +5972,7 @@
         <v>17</v>
       </c>
       <c r="AC24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AF24" s="17">
         <v>0</v>
@@ -6075,12 +5998,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="L25" s="6">
         <v>0</v>
@@ -6101,7 +6024,7 @@
         <v>23</v>
       </c>
       <c r="AC25" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AF25" s="17">
         <v>0</v>
@@ -6126,12 +6049,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -6149,10 +6072,10 @@
         <v>1</v>
       </c>
       <c r="AB26" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="AC26" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="AF26" s="17">
         <v>0</v>
@@ -6177,18 +6100,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="AR27" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AS27" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G28" s="5" t="s">
         <v>19</v>
       </c>
@@ -6200,7 +6123,7 @@
         <v>20</v>
       </c>
       <c r="AC28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AF28" s="17">
         <f>SUM(AF23:AF25)</f>
@@ -6226,22 +6149,22 @@
         <f>SUM(_xlfn.ANCHORARRAY(AL23))</f>
         <v>150</v>
       </c>
-      <c r="AN28" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO28" s="23">
+      <c r="AN28" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO28" s="22">
         <f>SUM(AO23:AO26)/(SUM(AF28:AJ28)+AL28)</f>
         <v>1</v>
       </c>
-      <c r="AR28" s="24">
+      <c r="AR28" s="23">
         <f>SUM(AF28:AJ28)+AL28</f>
         <v>150</v>
       </c>
-      <c r="AS28" s="25">
+      <c r="AS28" s="24">
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="2:45" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:45" x14ac:dyDescent="0.25">
       <c r="G29" s="12">
         <v>0</v>
       </c>
@@ -6271,37 +6194,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="M30" s="8"/>
-      <c r="N30" s="47" t="s">
-        <v>78</v>
+      <c r="N30" s="46" t="s">
+        <v>70</v>
       </c>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
-      <c r="AA30" s="33"/>
-      <c r="AB30" s="34"/>
-      <c r="AC30" s="34"/>
-      <c r="AD30" s="34"/>
-      <c r="AE30" s="34"/>
-      <c r="AF30" s="34"/>
-      <c r="AG30" s="34"/>
-      <c r="AH30" s="34"/>
-      <c r="AI30" s="34"/>
-      <c r="AJ30" s="34"/>
-      <c r="AK30" s="34"/>
-      <c r="AL30" s="34"/>
-      <c r="AM30" s="34"/>
-      <c r="AN30" s="34"/>
-      <c r="AO30" s="34"/>
-      <c r="AP30" s="34"/>
-      <c r="AQ30" s="34"/>
-      <c r="AR30" s="35"/>
-    </row>
-    <row r="31" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA30" s="32"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="33"/>
+      <c r="AD30" s="33"/>
+      <c r="AE30" s="33"/>
+      <c r="AF30" s="33"/>
+      <c r="AG30" s="33"/>
+      <c r="AH30" s="33"/>
+      <c r="AI30" s="33"/>
+      <c r="AJ30" s="33"/>
+      <c r="AK30" s="33"/>
+      <c r="AL30" s="33"/>
+      <c r="AM30" s="33"/>
+      <c r="AN30" s="33"/>
+      <c r="AO30" s="33"/>
+      <c r="AP30" s="33"/>
+      <c r="AQ30" s="33"/>
+      <c r="AR30" s="34"/>
+    </row>
+    <row r="31" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -6309,70 +6232,70 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
-      <c r="O31" s="51">
+      <c r="O31" s="50">
         <f>AC15*AR18</f>
         <v>0</v>
       </c>
       <c r="P31" s="18"/>
       <c r="R31" s="5"/>
-      <c r="AA31" s="36" t="s">
-        <v>70</v>
+      <c r="AA31" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
       <c r="AD31" s="5"/>
       <c r="AE31" s="5"/>
-      <c r="AR31" s="37"/>
-    </row>
-    <row r="32" spans="2:45" x14ac:dyDescent="0.35">
+      <c r="AR31" s="36"/>
+    </row>
+    <row r="32" spans="2:45" x14ac:dyDescent="0.25">
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="L32" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
-      <c r="AA32" s="38"/>
+      <c r="AA32" s="37"/>
       <c r="AN32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AQ32" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR32" s="39"/>
-    </row>
-    <row r="33" spans="7:44" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="AR32" s="38"/>
+    </row>
+    <row r="33" spans="7:44" x14ac:dyDescent="0.25">
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
-      <c r="L33" s="21">
+      <c r="L33" s="20">
         <v>1</v>
       </c>
-      <c r="M33" s="21">
-        <v>0</v>
-      </c>
-      <c r="N33" s="21">
-        <v>0</v>
-      </c>
-      <c r="O33" s="21">
-        <v>0</v>
-      </c>
-      <c r="P33" s="21">
+      <c r="M33" s="20">
+        <v>0</v>
+      </c>
+      <c r="N33" s="20">
+        <v>0</v>
+      </c>
+      <c r="O33" s="20">
+        <v>0</v>
+      </c>
+      <c r="P33" s="20">
         <v>0</v>
       </c>
       <c r="R33" s="8"/>
       <c r="X33" s="5"/>
-      <c r="AA33" s="38"/>
+      <c r="AA33" s="37"/>
       <c r="AB33" t="s">
         <v>16</v>
       </c>
       <c r="AC33" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AF33" s="17">
         <f>AF23</f>
@@ -6399,13 +6322,13 @@
         <f>SUM(AF33:AL33)</f>
         <v>150</v>
       </c>
-      <c r="AQ33" s="45" t="e">
+      <c r="AQ33" s="44" t="e">
         <f>(G19*N29+H19*O29)/(N29+O29)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AR33" s="37"/>
-    </row>
-    <row r="34" spans="7:44" x14ac:dyDescent="0.35">
+      <c r="AR33" s="36"/>
+    </row>
+    <row r="34" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L34" s="13">
         <v>0</v>
       </c>
@@ -6422,12 +6345,12 @@
         <v>0</v>
       </c>
       <c r="R34" s="8"/>
-      <c r="AA34" s="38"/>
+      <c r="AA34" s="37"/>
       <c r="AB34" t="s">
         <v>17</v>
       </c>
       <c r="AC34" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AF34" s="17">
         <f>AF24</f>
@@ -6451,9 +6374,9 @@
         <f t="shared" ref="AN34:AN35" si="0">SUM(AF34:AL34)</f>
         <v>0</v>
       </c>
-      <c r="AR34" s="37"/>
-    </row>
-    <row r="35" spans="7:44" x14ac:dyDescent="0.35">
+      <c r="AR34" s="36"/>
+    </row>
+    <row r="35" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L35" s="13">
         <v>0</v>
       </c>
@@ -6470,12 +6393,12 @@
         <v>0</v>
       </c>
       <c r="R35" s="8"/>
-      <c r="AA35" s="38"/>
+      <c r="AA35" s="37"/>
       <c r="AB35" t="s">
         <v>23</v>
       </c>
       <c r="AC35" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AF35" s="17">
         <v>0</v>
@@ -6497,9 +6420,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AR35" s="37"/>
-    </row>
-    <row r="36" spans="7:44" x14ac:dyDescent="0.35">
+      <c r="AR35" s="36"/>
+    </row>
+    <row r="36" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L36" s="13">
         <v>0</v>
       </c>
@@ -6516,20 +6439,20 @@
         <v>1</v>
       </c>
       <c r="R36" s="8"/>
-      <c r="AA36" s="38"/>
+      <c r="AA36" s="37"/>
       <c r="AQ36" s="5"/>
-      <c r="AR36" s="39"/>
-    </row>
-    <row r="37" spans="7:44" x14ac:dyDescent="0.35">
+      <c r="AR36" s="38"/>
+    </row>
+    <row r="37" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
       <c r="R37" s="8"/>
-      <c r="AA37" s="38"/>
+      <c r="AA37" s="37"/>
       <c r="AE37" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="AF37" s="17">
         <f>SUM(AF33:AF35)</f>
@@ -6556,69 +6479,69 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AM37" s="27"/>
-      <c r="AN37" s="26"/>
-      <c r="AR37" s="40"/>
-    </row>
-    <row r="38" spans="7:44" x14ac:dyDescent="0.35">
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="42"/>
-      <c r="AC38" s="42"/>
-      <c r="AD38" s="42"/>
-      <c r="AE38" s="42"/>
-      <c r="AF38" s="42"/>
-      <c r="AG38" s="42"/>
-      <c r="AH38" s="42"/>
-      <c r="AI38" s="42"/>
-      <c r="AJ38" s="42"/>
-      <c r="AK38" s="42"/>
-      <c r="AL38" s="42"/>
-      <c r="AM38" s="42"/>
-      <c r="AN38" s="42"/>
-      <c r="AO38" s="42"/>
-      <c r="AP38" s="42"/>
-      <c r="AQ38" s="42"/>
-      <c r="AR38" s="43"/>
-    </row>
-    <row r="39" spans="7:44" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM37" s="26"/>
+      <c r="AN37" s="25"/>
+      <c r="AR37" s="39"/>
+    </row>
+    <row r="38" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="AA38" s="40"/>
+      <c r="AB38" s="41"/>
+      <c r="AC38" s="41"/>
+      <c r="AD38" s="41"/>
+      <c r="AE38" s="41"/>
+      <c r="AF38" s="41"/>
+      <c r="AG38" s="41"/>
+      <c r="AH38" s="41"/>
+      <c r="AI38" s="41"/>
+      <c r="AJ38" s="41"/>
+      <c r="AK38" s="41"/>
+      <c r="AL38" s="41"/>
+      <c r="AM38" s="41"/>
+      <c r="AN38" s="41"/>
+      <c r="AO38" s="41"/>
+      <c r="AP38" s="41"/>
+      <c r="AQ38" s="41"/>
+      <c r="AR38" s="42"/>
+    </row>
+    <row r="39" spans="7:44" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q39" s="5"/>
       <c r="R39" s="9"/>
-      <c r="S39" s="54"/>
-      <c r="T39" s="54"/>
-    </row>
-    <row r="42" spans="7:44" x14ac:dyDescent="0.35">
+      <c r="S39" s="53"/>
+      <c r="T39" s="53"/>
+    </row>
+    <row r="42" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
     </row>
-    <row r="43" spans="7:44" x14ac:dyDescent="0.35">
+    <row r="43" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
     </row>
-    <row r="44" spans="7:44" x14ac:dyDescent="0.35">
+    <row r="44" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
     </row>
-    <row r="45" spans="7:44" x14ac:dyDescent="0.35">
+    <row r="45" spans="7:44" x14ac:dyDescent="0.25">
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
     </row>
-    <row r="47" spans="7:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="54"/>
+    <row r="47" spans="7:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L47" s="53"/>
+      <c r="M47" s="53"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="53"/>
       <c r="P47" s="9"/>
       <c r="R47" s="5"/>
     </row>
@@ -6634,26 +6557,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c319d79e-6821-4c2a-8db8-88a02643e5e3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa97a2c6-5066-49ad-90c0-e23f9da31bb2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D81D9CE2A426814A9054AC6C4C722ED5" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="df56dec458b733a6f5a4aa88128e48ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aa97a2c6-5066-49ad-90c0-e23f9da31bb2" xmlns:ns3="c319d79e-6821-4c2a-8db8-88a02643e5e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57b3dd0920a9f069281dfcd1579251e0" ns2:_="" ns3:_="">
     <xsd:import namespace="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
@@ -6842,26 +6745,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{244CEDEF-44DB-4344-910C-A3D03FE42352}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c319d79e-6821-4c2a-8db8-88a02643e5e3"/>
-    <ds:schemaRef ds:uri="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0520C8-B306-4A76-8642-CA302DC3B374}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c319d79e-6821-4c2a-8db8-88a02643e5e3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa97a2c6-5066-49ad-90c0-e23f9da31bb2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AD8AFD-ADBA-4FFD-B454-52613AC5E6B1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6878,4 +6782,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0520C8-B306-4A76-8642-CA302DC3B374}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{244CEDEF-44DB-4344-910C-A3D03FE42352}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c319d79e-6821-4c2a-8db8-88a02643e5e3"/>
+    <ds:schemaRef ds:uri="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>